<commit_message>
Updated alignments and MSA hierarchy.
</commit_message>
<xml_diff>
--- a/tabular/aav-refseqs-taxonomy.xlsx
+++ b/tabular/aav-refseqs-taxonomy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/gene-therapy/AAV-Atlas/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8DEEF574-E803-3A46-BE69-AB3AE9A1EB11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A484EA8D-4B32-9347-A787-4BECAB7E8595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="500" windowWidth="27580" windowHeight="16940"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="27980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aav-refseqs-taxonomy" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>sequenceID</t>
   </si>
@@ -176,12 +176,15 @@
   </si>
   <si>
     <t>Rodent1</t>
+  </si>
+  <si>
+    <t>MgAAV2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1022,11 +1025,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="A1:C23"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,7 +1284,7 @@
         <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Taxonomy consistent with ICTV
</commit_message>
<xml_diff>
--- a/tabular/aav-refseqs-taxonomy.xlsx
+++ b/tabular/aav-refseqs-taxonomy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/gene-therapy/AAV-Atlas/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D5581F-E90C-8F48-BC5B-46B4799A0F32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D599FB54-1CF0-BF49-9E73-E5BA61B7BC67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="2540" windowWidth="27980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aav-refseqs-taxonomy" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>sequenceID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>AAV1</t>
   </si>
   <si>
-    <t>DependoA</t>
-  </si>
-  <si>
     <t>NC_001401</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>AAV5</t>
   </si>
   <si>
-    <t>DependoB</t>
-  </si>
-  <si>
     <t>DQ335246</t>
   </si>
   <si>
@@ -133,18 +127,12 @@
     <t>BatAAV</t>
   </si>
   <si>
-    <t>Bat</t>
-  </si>
-  <si>
     <t>NC_038539</t>
   </si>
   <si>
     <t>PinAAV</t>
   </si>
   <si>
-    <t>Carnivore</t>
-  </si>
-  <si>
     <t>MN242366</t>
   </si>
   <si>
@@ -179,6 +167,60 @@
   </si>
   <si>
     <t>serotype</t>
+  </si>
+  <si>
+    <t>Primate1</t>
+  </si>
+  <si>
+    <t>Mammalian1</t>
+  </si>
+  <si>
+    <t>GenBank Refseq</t>
+  </si>
+  <si>
+    <t>GU226971</t>
+  </si>
+  <si>
+    <t>MG745677</t>
+  </si>
+  <si>
+    <t>Chiropteran1</t>
+  </si>
+  <si>
+    <t>Chiropteran2</t>
+  </si>
+  <si>
+    <t>DrAAV</t>
+  </si>
+  <si>
+    <t>JN420372</t>
+  </si>
+  <si>
+    <t>AF063497</t>
+  </si>
+  <si>
+    <t>AF043303</t>
+  </si>
+  <si>
+    <t>U48704</t>
+  </si>
+  <si>
+    <t>U89790</t>
+  </si>
+  <si>
+    <t>AF513851</t>
+  </si>
+  <si>
+    <t>AF513852</t>
+  </si>
+  <si>
+    <t>AF085716</t>
+  </si>
+  <si>
+    <t>AY388617</t>
+  </si>
+  <si>
+    <t>Carnivore1</t>
   </si>
 </sst>
 </file>
@@ -1026,15 +1068,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C23"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,255 +1089,299 @@
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C23">
-    <sortCondition ref="B2:B23"/>
-    <sortCondition ref="C2:C23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
+    <sortCondition ref="C2:C24"/>
+    <sortCondition ref="D2:D24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Gene recogniser set up
</commit_message>
<xml_diff>
--- a/tabular/aav-refseqs-taxonomy.xlsx
+++ b/tabular/aav-refseqs-taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/gene-therapy/AAV-Atlas/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0485D5EE-A9C8-F44E-AC61-8A2CD6946F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66825B4C-152A-4648-96D7-60DAB74417D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="27940" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,9 +716,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1071,7 +1078,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1096,285 +1103,298 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Materials supporting reproduction of AAV capsid horizontal transfer analysis
</commit_message>
<xml_diff>
--- a/tabular/aav-refseqs-taxonomy.xlsx
+++ b/tabular/aav-refseqs-taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/gene-therapy/AAV-Atlas/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66825B4C-152A-4648-96D7-60DAB74417D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643998A-9834-C547-B82B-7BB388D18BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="27940" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
   <si>
     <t>sequenceID</t>
   </si>
@@ -221,6 +221,129 @@
   </si>
   <si>
     <t>Carnivore1</t>
+  </si>
+  <si>
+    <t>KP733794</t>
+  </si>
+  <si>
+    <t>NC_027429</t>
+  </si>
+  <si>
+    <t>Bearded dragon parvovirus strain 2014</t>
+  </si>
+  <si>
+    <t>BdPV</t>
+  </si>
+  <si>
+    <t>full name</t>
+  </si>
+  <si>
+    <t>Bat adeno-associated virus</t>
+  </si>
+  <si>
+    <t>Desmodus rotundus dependoparvovirus isolate 246</t>
+  </si>
+  <si>
+    <t>NC_006148</t>
+  </si>
+  <si>
+    <t>California sea lion adeno-associated virus 1 isolate 1187</t>
+  </si>
+  <si>
+    <t>Snake parvovirus 1</t>
+  </si>
+  <si>
+    <t>SnPv</t>
+  </si>
+  <si>
+    <t>AY349010</t>
+  </si>
+  <si>
+    <t>AvAAV-ATCC-VR-865</t>
+  </si>
+  <si>
+    <t>AY186198</t>
+  </si>
+  <si>
+    <t>AY629583</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 10</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 11</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 12</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 2</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 3</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 4</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 6</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 7</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 8</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 9</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 5</t>
+  </si>
+  <si>
+    <t>Avian adeno-associated virus ATCC VR-865</t>
+  </si>
+  <si>
+    <t>Avian adeno-associated virus strain DA-1</t>
+  </si>
+  <si>
+    <t>AvAAV-DA-1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus isolate MgAAV2</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus isolate MgAAV1</t>
+  </si>
+  <si>
+    <t>Murine adeno-associated virus 1 isolate MAAV1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus - Po1</t>
+  </si>
+  <si>
+    <t>Bovine adeno-associated virus</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus-Go.1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus isolate MCAAV1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus isolate MCAAV2</t>
+  </si>
+  <si>
+    <t>Reptile1</t>
+  </si>
+  <si>
+    <t>Reptile2</t>
+  </si>
+  <si>
+    <t>Galliformes1</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,9 +1209,11 @@
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1101,8 +1226,11 @@
       <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
@@ -1115,8 +1243,11 @@
       <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -1127,8 +1258,11 @@
       <c r="D3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -1141,8 +1275,11 @@
       <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -1155,8 +1292,11 @@
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1167,8 +1307,11 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1179,8 +1322,11 @@
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1191,8 +1337,11 @@
       <c r="D8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
@@ -1205,8 +1354,11 @@
       <c r="D9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>60</v>
       </c>
@@ -1219,8 +1371,11 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1233,8 +1388,11 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1245,8 +1403,11 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -1259,8 +1420,11 @@
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1273,8 +1437,11 @@
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1285,8 +1452,11 @@
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -1299,8 +1469,11 @@
       <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1311,8 +1484,11 @@
       <c r="D17" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
@@ -1325,8 +1501,11 @@
       <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1337,8 +1516,11 @@
       <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1349,8 +1531,11 @@
       <c r="D20" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1361,8 +1546,11 @@
       <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -1373,8 +1561,11 @@
       <c r="D22" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>37</v>
       </c>
@@ -1385,8 +1576,11 @@
       <c r="D23" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -1396,6 +1590,73 @@
       </c>
       <c r="D24" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring for reproducibility of HT analysis paper
</commit_message>
<xml_diff>
--- a/tabular/aav-refseqs-taxonomy.xlsx
+++ b/tabular/aav-refseqs-taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/gene-therapy/AAV-Atlas/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643998A-9834-C547-B82B-7BB388D18BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF934411-BE90-9F4D-AB6E-85585DAEBE57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="27940" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>sequenceID</t>
   </si>
@@ -181,18 +181,9 @@
     <t>GU226971</t>
   </si>
   <si>
-    <t>MG745677</t>
-  </si>
-  <si>
     <t>Chiropteran1</t>
   </si>
   <si>
-    <t>Chiropteran2</t>
-  </si>
-  <si>
-    <t>DrAAV</t>
-  </si>
-  <si>
     <t>JN420372</t>
   </si>
   <si>
@@ -223,51 +214,15 @@
     <t>Carnivore1</t>
   </si>
   <si>
-    <t>KP733794</t>
-  </si>
-  <si>
-    <t>NC_027429</t>
-  </si>
-  <si>
-    <t>Bearded dragon parvovirus strain 2014</t>
-  </si>
-  <si>
-    <t>BdPV</t>
-  </si>
-  <si>
     <t>full name</t>
   </si>
   <si>
     <t>Bat adeno-associated virus</t>
   </si>
   <si>
-    <t>Desmodus rotundus dependoparvovirus isolate 246</t>
-  </si>
-  <si>
-    <t>NC_006148</t>
-  </si>
-  <si>
     <t>California sea lion adeno-associated virus 1 isolate 1187</t>
   </si>
   <si>
-    <t>Snake parvovirus 1</t>
-  </si>
-  <si>
-    <t>SnPv</t>
-  </si>
-  <si>
-    <t>AY349010</t>
-  </si>
-  <si>
-    <t>AvAAV-ATCC-VR-865</t>
-  </si>
-  <si>
-    <t>AY186198</t>
-  </si>
-  <si>
-    <t>AY629583</t>
-  </si>
-  <si>
     <t>Adeno-associated virus 1</t>
   </si>
   <si>
@@ -304,15 +259,6 @@
     <t>Adeno-associated virus 5</t>
   </si>
   <si>
-    <t>Avian adeno-associated virus ATCC VR-865</t>
-  </si>
-  <si>
-    <t>Avian adeno-associated virus strain DA-1</t>
-  </si>
-  <si>
-    <t>AvAAV-DA-1</t>
-  </si>
-  <si>
     <t>Adeno-associated virus isolate MgAAV2</t>
   </si>
   <si>
@@ -335,15 +281,6 @@
   </si>
   <si>
     <t>Adeno-associated virus isolate MCAAV2</t>
-  </si>
-  <si>
-    <t>Reptile1</t>
-  </si>
-  <si>
-    <t>Reptile2</t>
-  </si>
-  <si>
-    <t>Galliformes1</t>
   </si>
 </sst>
 </file>
@@ -1198,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,7 +1164,7 @@
         <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,431 +1175,352 @@
         <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>95</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
-    <sortCondition ref="C2:C24"/>
-    <sortCondition ref="D2:D24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
+    <sortCondition ref="C2:C23"/>
+    <sortCondition ref="D2:D23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>